<commit_message>
Add signal quality queries/parsing.
</commit_message>
<xml_diff>
--- a/metars.xlsx
+++ b/metars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
   <si>
     <t>Timstamp (hour) - 5 bits</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>&gt;5ºC</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -396,6 +399,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -768,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G206"/>
+  <dimension ref="A1:G207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,7 +795,7 @@
         <v>24</v>
       </c>
       <c r="E1">
-        <f>SUM(C1:C82)</f>
+        <f>SUM(C1:C83)</f>
         <v>61</v>
       </c>
       <c r="G1">
@@ -1177,11 +1183,11 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>48</v>
+      <c r="B50" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1189,7 +1195,7 @@
         <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1197,7 +1203,7 @@
         <v>25</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1205,7 +1211,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1213,7 +1219,7 @@
         <v>28</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1221,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1229,7 +1235,7 @@
         <v>62</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1237,7 +1243,7 @@
         <v>63</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1245,7 +1251,7 @@
         <v>15</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1253,7 +1259,7 @@
         <v>64</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1261,7 +1267,7 @@
         <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1269,7 +1275,7 @@
         <v>66</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1277,7 +1283,7 @@
         <v>67</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1285,159 +1291,163 @@
         <v>68</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64">
+      <c r="B65" s="2"/>
+      <c r="C65">
         <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="2"/>
-      <c r="C68">
+      <c r="B69" s="2"/>
+      <c r="C69">
         <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="1">
-        <v>4</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1">
+        <v>6</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
         <v>7</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:3">
+      <c r="A78" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B77" s="2"/>
-      <c r="C77">
+      <c r="B78" s="2"/>
+      <c r="C78">
         <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1"/>
@@ -1935,10 +1945,14 @@
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
     </row>
+    <row r="207" spans="1:2">
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A78:B78"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A13:B13"/>
@@ -1948,7 +1962,7 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update METAR encoding spec.
</commit_message>
<xml_diff>
--- a/metars.xlsx
+++ b/metars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
   <si>
     <t>Timstamp (hour) - 5 bits</t>
   </si>
@@ -288,10 +288,22 @@
     <t>Location Identifier - 24 bits</t>
   </si>
   <si>
-    <t>&gt;5ºC</t>
-  </si>
-  <si>
     <t>14</t>
+  </si>
+  <si>
+    <t>Notification - 1 bit</t>
+  </si>
+  <si>
+    <t>Request full METAR for further info</t>
+  </si>
+  <si>
+    <t>5ºC</t>
+  </si>
+  <si>
+    <t>6ºC</t>
+  </si>
+  <si>
+    <t>&gt;=7ºC</t>
   </si>
 </sst>
 </file>
@@ -331,12 +343,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -391,18 +409,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -774,734 +797,777 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G207"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
       <c r="C1">
         <v>24</v>
       </c>
       <c r="E1">
-        <f>SUM(C1:C83)</f>
-        <v>61</v>
+        <f>SUM(C1:C85)</f>
+        <v>62</v>
       </c>
       <c r="G1">
         <f>400/E1</f>
-        <v>6.557377049180328</v>
+        <v>6.4516129032258061</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1">
+      <c r="A6" s="7">
         <v>23</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1">
+      <c r="A8" s="7">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1">
+      <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1">
+      <c r="A10" s="7">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1">
+      <c r="A12" s="7">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="1">
+      <c r="A14" s="7">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="1">
+      <c r="A15" s="7">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="1">
+      <c r="A16" s="7">
         <v>2</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17" s="7">
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18" s="7">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="B19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
+    <row r="23" spans="1:3">
+      <c r="A23" s="7">
         <v>0</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B24" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>7</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26">
+      <c r="B28" s="3"/>
+      <c r="C28">
         <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2" t="s">
+    <row r="33" spans="1:3">
+      <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31">
+      <c r="B33" s="3"/>
+      <c r="C33">
         <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1">
-        <v>1</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
         <v>3</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36">
+      <c r="B38" s="3"/>
+      <c r="C38">
         <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41">
-        <v>6</v>
+      <c r="A41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>42</v>
+      <c r="A43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43">
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="1">
-        <v>62</v>
+      <c r="A47" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>62</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="2" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49">
+      <c r="B51" s="3"/>
+      <c r="C51">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65">
-        <v>2</v>
+      <c r="A65" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>72</v>
+      <c r="A67" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67">
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69">
-        <v>3</v>
+      <c r="A69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>75</v>
+      <c r="A71" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71">
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1">
-        <v>4</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="1">
-        <v>5</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1">
+        <v>5</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>6</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
         <v>7</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="2" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B78" s="2"/>
-      <c r="C78">
+      <c r="B80" s="3"/>
+      <c r="C80">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="1" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="1:2">
+    <row r="85" spans="1:3">
+      <c r="A85" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
     </row>
@@ -1949,20 +2015,29 @@
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
     </row>
+    <row r="208" spans="1:2">
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" s="1"/>
+      <c r="B209" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A78:B78"/>
+  <mergeCells count="14">
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A80:B80"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>